<commit_message>
Enhance email automation with attachments and smooth workflow scripts
</commit_message>
<xml_diff>
--- a/output/scans/calstatela-edu_accessibility/calstatela-pdf-scans.xlsx
+++ b/output/scans/calstatela-edu_accessibility/calstatela-pdf-scans.xlsx
@@ -583,7 +583,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-11-03 20:04:47</t>
+          <t>2025-12-16 19:09:44</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-11-03 20:04:58</t>
+          <t>2025-12-16 19:10:07</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -751,7 +751,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-11-03 20:04:59</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -826,21 +826,21 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/Renewed%20Campus%20Commitment%20ATI_103024.pdf", "https://www.calstatela.edu/sites/default/files/Renewed%20Campus%20Commitment%20ATI_103024.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B5" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ada-title-ii-update", "https://www.calstatela.edu/accessibility/ada-title-ii-update")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/documents", "https://www.calstatela.edu/accessibility/documents")</f>
         <v/>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:00</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>c58a0e</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -857,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
@@ -910,21 +910,21 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B6" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ada-title-ii-update", "https://www.calstatela.edu/accessibility/ada-title-ii-update")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/documents", "https://www.calstatela.edu/accessibility/documents")</f>
         <v/>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:00</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -941,7 +941,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
@@ -994,21 +994,21 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B7" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ada-title-ii-update", "https://www.calstatela.edu/accessibility/ada-title-ii-update")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/audio-and-video", "https://www.calstatela.edu/accessibility/audio-and-video")</f>
         <v/>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:00</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1025,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -1054,7 +1054,7 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
@@ -1063,7 +1063,7 @@
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
@@ -1078,21 +1078,21 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B8" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/portal-accessibility", "https://www.calstatela.edu/accessibility/portal-accessibility")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/audio-and-video", "https://www.calstatela.edu/accessibility/audio-and-video")</f>
         <v/>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:00</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1109,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -1138,7 +1138,7 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
@@ -1147,7 +1147,7 @@
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
@@ -1162,21 +1162,21 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B9" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/portal-accessibility", "https://www.calstatela.edu/accessibility/portal-accessibility")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/udoit", "https://www.calstatela.edu/accessibility/udoit")</f>
         <v/>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:00</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1193,7 +1193,7 @@
         <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
         <v>0</v>
@@ -1231,7 +1231,7 @@
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -1246,21 +1246,21 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B10" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessibility-statement", "https://www.calstatela.edu/accessibility/accessibility-statement")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/udoit", "https://www.calstatela.edu/accessibility/udoit")</f>
         <v/>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:00</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1277,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1306,7 +1306,7 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10" t="n">
         <v>0</v>
@@ -1315,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
@@ -1330,21 +1330,21 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B11" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessibility-statement", "https://www.calstatela.edu/accessibility/accessibility-statement")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/new-faculty", "https://www.calstatela.edu/accessibility/new-faculty")</f>
         <v/>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:00</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
         <v>0</v>
@@ -1399,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
@@ -1414,21 +1414,21 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/ati_handout_021721.pdf", "https://www.calstatela.edu/sites/default/files/ati_handout_021721.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B12" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessibility-primer", "https://www.calstatela.edu/accessibility/accessibility-primer")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/new-faculty", "https://www.calstatela.edu/accessibility/new-faculty")</f>
         <v/>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>9f5e7f</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1470,11 +1470,11 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12" t="n">
         <v>0</v>
@@ -1502,12 +1502,12 @@
         <v/>
       </c>
       <c r="B13" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessibility-primer", "https://www.calstatela.edu/accessibility/accessibility-primer")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/instructional-materials", "https://www.calstatela.edu/accessibility/instructional-materials")</f>
         <v/>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1586,12 +1586,12 @@
         <v/>
       </c>
       <c r="B14" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessibility-primer", "https://www.calstatela.edu/accessibility/accessibility-primer")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/instructional-materials", "https://www.calstatela.edu/accessibility/instructional-materials")</f>
         <v/>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1670,12 +1670,12 @@
         <v/>
       </c>
       <c r="B15" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/frequently-asked-questions", "https://www.calstatela.edu/accessibility/frequently-asked-questions")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/seven-essential-skills-crafting-accessible-content", "https://www.calstatela.edu/accessibility/seven-essential-skills-crafting-accessible-content")</f>
         <v/>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1754,12 +1754,12 @@
         <v/>
       </c>
       <c r="B16" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/frequently-asked-questions", "https://www.calstatela.edu/accessibility/frequently-asked-questions")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/seven-essential-skills-crafting-accessible-content", "https://www.calstatela.edu/accessibility/seven-essential-skills-crafting-accessible-content")</f>
         <v/>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1838,12 +1838,12 @@
         <v/>
       </c>
       <c r="B17" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/campus-resources", "https://www.calstatela.edu/accessibility/campus-resources")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/editoria11y-drupal", "https://www.calstatela.edu/accessibility/editoria11y-drupal")</f>
         <v/>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1922,12 +1922,12 @@
         <v/>
       </c>
       <c r="B18" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/campus-resources", "https://www.calstatela.edu/accessibility/campus-resources")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/editoria11y-drupal", "https://www.calstatela.edu/accessibility/editoria11y-drupal")</f>
         <v/>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2006,12 +2006,12 @@
         <v/>
       </c>
       <c r="B19" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/cetl", "https://www.calstatela.edu/accessibility/cetl")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/popetech-wave", "https://www.calstatela.edu/accessibility/popetech-wave")</f>
         <v/>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2090,12 +2090,12 @@
         <v/>
       </c>
       <c r="B20" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/cetl", "https://www.calstatela.edu/accessibility/cetl")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/popetech-wave", "https://www.calstatela.edu/accessibility/popetech-wave")</f>
         <v/>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2174,12 +2174,12 @@
         <v/>
       </c>
       <c r="B21" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/digital-content-challenge", "https://www.calstatela.edu/accessibility/digital-content-challenge")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web-accessibility-guidelines", "https://www.calstatela.edu/accessibility/web-accessibility-guidelines")</f>
         <v/>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2258,12 +2258,12 @@
         <v/>
       </c>
       <c r="B22" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/digital-content-challenge", "https://www.calstatela.edu/accessibility/digital-content-challenge")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web-accessibility-guidelines", "https://www.calstatela.edu/accessibility/web-accessibility-guidelines")</f>
         <v/>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2342,12 +2342,12 @@
         <v/>
       </c>
       <c r="B23" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/systemwide-resources", "https://www.calstatela.edu/accessibility/systemwide-resources")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web-accessibility-liaisons", "https://www.calstatela.edu/accessibility/web-accessibility-liaisons")</f>
         <v/>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2426,12 +2426,12 @@
         <v/>
       </c>
       <c r="B24" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/systemwide-resources", "https://www.calstatela.edu/accessibility/systemwide-resources")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web-accessibility-liaisons", "https://www.calstatela.edu/accessibility/web-accessibility-liaisons")</f>
         <v/>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2510,12 +2510,12 @@
         <v/>
       </c>
       <c r="B25" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-intranet", "https://www.calstatela.edu/accessibility/ati-intranet")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ramp", "https://www.calstatela.edu/accessibility/ramp")</f>
         <v/>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2594,12 +2594,12 @@
         <v/>
       </c>
       <c r="B26" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-intranet", "https://www.calstatela.edu/accessibility/ati-intranet")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ramp", "https://www.calstatela.edu/accessibility/ramp")</f>
         <v/>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2678,12 +2678,12 @@
         <v/>
       </c>
       <c r="B27" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-governance", "https://www.calstatela.edu/accessibility/ati-governance")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web", "https://www.calstatela.edu/accessibility/web")</f>
         <v/>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2762,12 +2762,12 @@
         <v/>
       </c>
       <c r="B28" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-governance", "https://www.calstatela.edu/accessibility/ati-governance")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web", "https://www.calstatela.edu/accessibility/web")</f>
         <v/>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2846,12 +2846,12 @@
         <v/>
       </c>
       <c r="B29" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-campus-plan", "https://www.calstatela.edu/accessibility/ati-campus-plan")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/services", "https://www.calstatela.edu/accessibility/services")</f>
         <v/>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2930,12 +2930,12 @@
         <v/>
       </c>
       <c r="B30" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-campus-plan", "https://www.calstatela.edu/accessibility/ati-campus-plan")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/services", "https://www.calstatela.edu/accessibility/services")</f>
         <v/>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:01</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -3010,21 +3010,21 @@
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/ati_memo_march_2021.pdf", "https://www.calstatela.edu/sites/default/files/ati_memo_march_2021.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B31" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati", "https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/report-accessibility-issue", "https://www.calstatela.edu/accessibility/report-accessibility-issue")</f>
         <v/>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>e92ee3</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -3094,21 +3094,21 @@
     </row>
     <row r="32">
       <c r="A32" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B32" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati", "https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/report-accessibility-issue", "https://www.calstatela.edu/accessibility/report-accessibility-issue")</f>
         <v/>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:10</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -3125,7 +3125,7 @@
         <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
@@ -3154,7 +3154,7 @@
         </is>
       </c>
       <c r="O32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q32" t="n">
         <v>0</v>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="S32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T32" t="inlineStr">
         <is>
@@ -3178,21 +3178,21 @@
     </row>
     <row r="33">
       <c r="A33" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/Renewed%20Campus%20Commitment%20ATI_103024.pdf", "https://www.calstatela.edu/sites/default/files/Renewed%20Campus%20Commitment%20ATI_103024.pdf")</f>
         <v/>
       </c>
       <c r="B33" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati", "https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ada-title-ii-update", "https://www.calstatela.edu/accessibility/ada-title-ii-update")</f>
         <v/>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>c58a0e</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -3209,7 +3209,7 @@
         <v>1</v>
       </c>
       <c r="H33" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -3238,7 +3238,7 @@
         </is>
       </c>
       <c r="O33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q33" t="n">
         <v>0</v>
@@ -3247,7 +3247,7 @@
         <v>0</v>
       </c>
       <c r="S33" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T33" t="inlineStr">
         <is>
@@ -3266,12 +3266,12 @@
         <v/>
       </c>
       <c r="B34" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/software-licensing", "https://www.calstatela.edu/accessibility/software-licensing")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ada-title-ii-update", "https://www.calstatela.edu/accessibility/ada-title-ii-update")</f>
         <v/>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -3350,12 +3350,12 @@
         <v/>
       </c>
       <c r="B35" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/software-licensing", "https://www.calstatela.edu/accessibility/software-licensing")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ada-title-ii-update", "https://www.calstatela.edu/accessibility/ada-title-ii-update")</f>
         <v/>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3434,12 +3434,12 @@
         <v/>
       </c>
       <c r="B36" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/adaptive-workstations-assistive-technology", "https://www.calstatela.edu/accessibility/adaptive-workstations-assistive-technology")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/portal-accessibility", "https://www.calstatela.edu/accessibility/portal-accessibility")</f>
         <v/>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3518,12 +3518,12 @@
         <v/>
       </c>
       <c r="B37" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/adaptive-workstations-assistive-technology", "https://www.calstatela.edu/accessibility/adaptive-workstations-assistive-technology")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/portal-accessibility", "https://www.calstatela.edu/accessibility/portal-accessibility")</f>
         <v/>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3602,12 +3602,12 @@
         <v/>
       </c>
       <c r="B38" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/training", "https://www.calstatela.edu/accessibility/training")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/digital-content-challenge", "https://www.calstatela.edu/accessibility/digital-content-challenge")</f>
         <v/>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3686,12 +3686,12 @@
         <v/>
       </c>
       <c r="B39" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/training", "https://www.calstatela.edu/accessibility/training")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/digital-content-challenge", "https://www.calstatela.edu/accessibility/digital-content-challenge")</f>
         <v/>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3770,12 +3770,12 @@
         <v/>
       </c>
       <c r="B40" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/dcc-sign", "https://www.calstatela.edu/accessibility/dcc-sign")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/cetl", "https://www.calstatela.edu/accessibility/cetl")</f>
         <v/>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3854,12 +3854,12 @@
         <v/>
       </c>
       <c r="B41" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/dcc-sign", "https://www.calstatela.edu/accessibility/dcc-sign")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/cetl", "https://www.calstatela.edu/accessibility/cetl")</f>
         <v/>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3938,12 +3938,12 @@
         <v/>
       </c>
       <c r="B42" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/digital-content-challenge-0", "https://www.calstatela.edu/accessibility/digital-content-challenge-0")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/systemwide-resources", "https://www.calstatela.edu/accessibility/systemwide-resources")</f>
         <v/>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -4022,12 +4022,12 @@
         <v/>
       </c>
       <c r="B43" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/digital-content-challenge-0", "https://www.calstatela.edu/accessibility/digital-content-challenge-0")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/systemwide-resources", "https://www.calstatela.edu/accessibility/systemwide-resources")</f>
         <v/>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -4106,12 +4106,12 @@
         <v/>
       </c>
       <c r="B44" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessible-event-planning", "https://www.calstatela.edu/accessibility/accessible-event-planning")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-intranet", "https://www.calstatela.edu/accessibility/ati-intranet")</f>
         <v/>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -4190,12 +4190,12 @@
         <v/>
       </c>
       <c r="B45" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessible-event-planning", "https://www.calstatela.edu/accessibility/accessible-event-planning")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-intranet", "https://www.calstatela.edu/accessibility/ati-intranet")</f>
         <v/>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -4274,12 +4274,12 @@
         <v/>
       </c>
       <c r="B46" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/temporary-alternate-access-planning", "https://www.calstatela.edu/accessibility/temporary-alternate-access-planning")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-governance", "https://www.calstatela.edu/accessibility/ati-governance")</f>
         <v/>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -4358,12 +4358,12 @@
         <v/>
       </c>
       <c r="B47" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/temporary-alternate-access-planning", "https://www.calstatela.edu/accessibility/temporary-alternate-access-planning")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-governance", "https://www.calstatela.edu/accessibility/ati-governance")</f>
         <v/>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -4442,12 +4442,12 @@
         <v/>
       </c>
       <c r="B48" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/acr-repository", "https://www.calstatela.edu/accessibility/acr-repository")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-campus-plan", "https://www.calstatela.edu/accessibility/ati-campus-plan")</f>
         <v/>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4526,12 +4526,12 @@
         <v/>
       </c>
       <c r="B49" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/acr-repository", "https://www.calstatela.edu/accessibility/acr-repository")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ati-campus-plan", "https://www.calstatela.edu/accessibility/ati-campus-plan")</f>
         <v/>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:14</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4606,21 +4606,21 @@
     </row>
     <row r="50">
       <c r="A50" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/ati_memo_march_2021.pdf", "https://www.calstatela.edu/sites/default/files/ati_memo_march_2021.pdf")</f>
         <v/>
       </c>
       <c r="B50" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/vendor-requirements", "https://www.calstatela.edu/accessibility/vendor-requirements")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati", "https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati")</f>
         <v/>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>e92ee3</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -4690,21 +4690,21 @@
     </row>
     <row r="51">
       <c r="A51" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B51" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/vendor-requirements", "https://www.calstatela.edu/accessibility/vendor-requirements")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati", "https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati")</f>
         <v/>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -4721,7 +4721,7 @@
         <v>1</v>
       </c>
       <c r="H51" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -4750,7 +4750,7 @@
         </is>
       </c>
       <c r="O51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q51" t="n">
         <v>0</v>
@@ -4759,7 +4759,7 @@
         <v>0</v>
       </c>
       <c r="S51" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T51" t="inlineStr">
         <is>
@@ -4774,21 +4774,21 @@
     </row>
     <row r="52">
       <c r="A52" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B52" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/submit-ict-par", "https://www.calstatela.edu/accessibility/submit-ict-par")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati", "https://www.calstatela.edu/accessibility/accessible-technology-initiative-ati")</f>
         <v/>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -4805,7 +4805,7 @@
         <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
@@ -4834,7 +4834,7 @@
         </is>
       </c>
       <c r="O52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q52" t="n">
         <v>0</v>
@@ -4843,7 +4843,7 @@
         <v>0</v>
       </c>
       <c r="S52" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T52" t="inlineStr">
         <is>
@@ -4858,21 +4858,21 @@
     </row>
     <row r="53">
       <c r="A53" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B53" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/submit-ict-par", "https://www.calstatela.edu/accessibility/submit-ict-par")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/software-licensing", "https://www.calstatela.edu/accessibility/software-licensing")</f>
         <v/>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -4889,7 +4889,7 @@
         <v>1</v>
       </c>
       <c r="H53" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
@@ -4918,7 +4918,7 @@
         </is>
       </c>
       <c r="O53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q53" t="n">
         <v>0</v>
@@ -4927,7 +4927,7 @@
         <v>0</v>
       </c>
       <c r="S53" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T53" t="inlineStr">
         <is>
@@ -4942,21 +4942,21 @@
     </row>
     <row r="54">
       <c r="A54" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B54" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ict-purchase-approval-request-ict-par-walkthrough", "https://www.calstatela.edu/accessibility/ict-purchase-approval-request-ict-par-walkthrough")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/software-licensing", "https://www.calstatela.edu/accessibility/software-licensing")</f>
         <v/>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -4973,7 +4973,7 @@
         <v>1</v>
       </c>
       <c r="H54" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
@@ -5002,7 +5002,7 @@
         </is>
       </c>
       <c r="O54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q54" t="n">
         <v>0</v>
@@ -5011,7 +5011,7 @@
         <v>0</v>
       </c>
       <c r="S54" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T54" t="inlineStr">
         <is>
@@ -5026,21 +5026,21 @@
     </row>
     <row r="55">
       <c r="A55" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B55" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ict-purchase-approval-request-ict-par-walkthrough", "https://www.calstatela.edu/accessibility/ict-purchase-approval-request-ict-par-walkthrough")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/adaptive-workstations-assistive-technology", "https://www.calstatela.edu/accessibility/adaptive-workstations-assistive-technology")</f>
         <v/>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -5057,7 +5057,7 @@
         <v>1</v>
       </c>
       <c r="H55" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
@@ -5086,7 +5086,7 @@
         </is>
       </c>
       <c r="O55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q55" t="n">
         <v>0</v>
@@ -5095,7 +5095,7 @@
         <v>0</v>
       </c>
       <c r="S55" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T55" t="inlineStr">
         <is>
@@ -5110,21 +5110,21 @@
     </row>
     <row r="56">
       <c r="A56" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B56" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/pre-approved-ict", "https://www.calstatela.edu/accessibility/pre-approved-ict")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/adaptive-workstations-assistive-technology", "https://www.calstatela.edu/accessibility/adaptive-workstations-assistive-technology")</f>
         <v/>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -5141,7 +5141,7 @@
         <v>1</v>
       </c>
       <c r="H56" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
@@ -5170,7 +5170,7 @@
         </is>
       </c>
       <c r="O56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q56" t="n">
         <v>0</v>
@@ -5179,7 +5179,7 @@
         <v>0</v>
       </c>
       <c r="S56" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T56" t="inlineStr">
         <is>
@@ -5194,21 +5194,21 @@
     </row>
     <row r="57">
       <c r="A57" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B57" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/pre-approved-ict", "https://www.calstatela.edu/accessibility/pre-approved-ict")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/training", "https://www.calstatela.edu/accessibility/training")</f>
         <v/>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -5225,7 +5225,7 @@
         <v>1</v>
       </c>
       <c r="H57" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
@@ -5254,7 +5254,7 @@
         </is>
       </c>
       <c r="O57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q57" t="n">
         <v>0</v>
@@ -5263,7 +5263,7 @@
         <v>0</v>
       </c>
       <c r="S57" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T57" t="inlineStr">
         <is>
@@ -5278,21 +5278,21 @@
     </row>
     <row r="58">
       <c r="A58" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B58" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/acquiring-accessible-ict", "https://www.calstatela.edu/accessibility/acquiring-accessible-ict")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/training", "https://www.calstatela.edu/accessibility/training")</f>
         <v/>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -5309,7 +5309,7 @@
         <v>1</v>
       </c>
       <c r="H58" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
@@ -5338,7 +5338,7 @@
         </is>
       </c>
       <c r="O58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q58" t="n">
         <v>0</v>
@@ -5347,7 +5347,7 @@
         <v>0</v>
       </c>
       <c r="S58" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T58" t="inlineStr">
         <is>
@@ -5362,21 +5362,21 @@
     </row>
     <row r="59">
       <c r="A59" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B59" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/acquiring-accessible-ict", "https://www.calstatela.edu/accessibility/acquiring-accessible-ict")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/dcc-sign", "https://www.calstatela.edu/accessibility/dcc-sign")</f>
         <v/>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -5393,7 +5393,7 @@
         <v>1</v>
       </c>
       <c r="H59" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
@@ -5422,7 +5422,7 @@
         </is>
       </c>
       <c r="O59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q59" t="n">
         <v>0</v>
@@ -5431,7 +5431,7 @@
         <v>0</v>
       </c>
       <c r="S59" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T59" t="inlineStr">
         <is>
@@ -5446,21 +5446,21 @@
     </row>
     <row r="60">
       <c r="A60" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B60" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/zoom-and-teams", "https://www.calstatela.edu/accessibility/zoom-and-teams")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/dcc-sign", "https://www.calstatela.edu/accessibility/dcc-sign")</f>
         <v/>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -5477,7 +5477,7 @@
         <v>1</v>
       </c>
       <c r="H60" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
@@ -5506,7 +5506,7 @@
         </is>
       </c>
       <c r="O60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q60" t="n">
         <v>0</v>
@@ -5515,7 +5515,7 @@
         <v>0</v>
       </c>
       <c r="S60" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T60" t="inlineStr">
         <is>
@@ -5530,21 +5530,21 @@
     </row>
     <row r="61">
       <c r="A61" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B61" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/zoom-and-teams", "https://www.calstatela.edu/accessibility/zoom-and-teams")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/digital-content-challenge-0", "https://www.calstatela.edu/accessibility/digital-content-challenge-0")</f>
         <v/>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -5561,7 +5561,7 @@
         <v>1</v>
       </c>
       <c r="H61" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
@@ -5590,7 +5590,7 @@
         </is>
       </c>
       <c r="O61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q61" t="n">
         <v>0</v>
@@ -5599,7 +5599,7 @@
         <v>0</v>
       </c>
       <c r="S61" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T61" t="inlineStr">
         <is>
@@ -5614,21 +5614,21 @@
     </row>
     <row r="62">
       <c r="A62" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B62" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/qualtrics", "https://www.calstatela.edu/accessibility/qualtrics")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/digital-content-challenge-0", "https://www.calstatela.edu/accessibility/digital-content-challenge-0")</f>
         <v/>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -5645,7 +5645,7 @@
         <v>1</v>
       </c>
       <c r="H62" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I62" t="inlineStr">
         <is>
@@ -5674,7 +5674,7 @@
         </is>
       </c>
       <c r="O62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q62" t="n">
         <v>0</v>
@@ -5683,7 +5683,7 @@
         <v>0</v>
       </c>
       <c r="S62" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T62" t="inlineStr">
         <is>
@@ -5698,21 +5698,21 @@
     </row>
     <row r="63">
       <c r="A63" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B63" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/qualtrics", "https://www.calstatela.edu/accessibility/qualtrics")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessible-event-planning", "https://www.calstatela.edu/accessibility/accessible-event-planning")</f>
         <v/>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -5729,7 +5729,7 @@
         <v>1</v>
       </c>
       <c r="H63" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
@@ -5758,7 +5758,7 @@
         </is>
       </c>
       <c r="O63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q63" t="n">
         <v>0</v>
@@ -5767,7 +5767,7 @@
         <v>0</v>
       </c>
       <c r="S63" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T63" t="inlineStr">
         <is>
@@ -5782,21 +5782,21 @@
     </row>
     <row r="64">
       <c r="A64" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B64" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/social-media", "https://www.calstatela.edu/accessibility/social-media")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessible-event-planning", "https://www.calstatela.edu/accessibility/accessible-event-planning")</f>
         <v/>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -5813,7 +5813,7 @@
         <v>1</v>
       </c>
       <c r="H64" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I64" t="inlineStr">
         <is>
@@ -5842,7 +5842,7 @@
         </is>
       </c>
       <c r="O64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q64" t="n">
         <v>0</v>
@@ -5851,7 +5851,7 @@
         <v>0</v>
       </c>
       <c r="S64" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T64" t="inlineStr">
         <is>
@@ -5866,21 +5866,21 @@
     </row>
     <row r="65">
       <c r="A65" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B65" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/social-media", "https://www.calstatela.edu/accessibility/social-media")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/temporary-alternate-access-planning", "https://www.calstatela.edu/accessibility/temporary-alternate-access-planning")</f>
         <v/>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -5897,7 +5897,7 @@
         <v>1</v>
       </c>
       <c r="H65" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I65" t="inlineStr">
         <is>
@@ -5926,7 +5926,7 @@
         </is>
       </c>
       <c r="O65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q65" t="n">
         <v>0</v>
@@ -5935,7 +5935,7 @@
         <v>0</v>
       </c>
       <c r="S65" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T65" t="inlineStr">
         <is>
@@ -5950,21 +5950,21 @@
     </row>
     <row r="66">
       <c r="A66" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B66" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/documents", "https://www.calstatela.edu/accessibility/documents")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/temporary-alternate-access-planning", "https://www.calstatela.edu/accessibility/temporary-alternate-access-planning")</f>
         <v/>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -5981,7 +5981,7 @@
         <v>1</v>
       </c>
       <c r="H66" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I66" t="inlineStr">
         <is>
@@ -6010,7 +6010,7 @@
         </is>
       </c>
       <c r="O66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q66" t="n">
         <v>0</v>
@@ -6019,7 +6019,7 @@
         <v>0</v>
       </c>
       <c r="S66" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T66" t="inlineStr">
         <is>
@@ -6034,21 +6034,21 @@
     </row>
     <row r="67">
       <c r="A67" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B67" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/documents", "https://www.calstatela.edu/accessibility/documents")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/acr-repository", "https://www.calstatela.edu/accessibility/acr-repository")</f>
         <v/>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -6065,7 +6065,7 @@
         <v>1</v>
       </c>
       <c r="H67" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I67" t="inlineStr">
         <is>
@@ -6094,7 +6094,7 @@
         </is>
       </c>
       <c r="O67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q67" t="n">
         <v>0</v>
@@ -6103,7 +6103,7 @@
         <v>0</v>
       </c>
       <c r="S67" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T67" t="inlineStr">
         <is>
@@ -6118,21 +6118,21 @@
     </row>
     <row r="68">
       <c r="A68" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B68" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/audio-and-video", "https://www.calstatela.edu/accessibility/audio-and-video")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/acr-repository", "https://www.calstatela.edu/accessibility/acr-repository")</f>
         <v/>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -6149,7 +6149,7 @@
         <v>1</v>
       </c>
       <c r="H68" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I68" t="inlineStr">
         <is>
@@ -6178,7 +6178,7 @@
         </is>
       </c>
       <c r="O68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q68" t="n">
         <v>0</v>
@@ -6187,7 +6187,7 @@
         <v>0</v>
       </c>
       <c r="S68" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T68" t="inlineStr">
         <is>
@@ -6202,21 +6202,21 @@
     </row>
     <row r="69">
       <c r="A69" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B69" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/audio-and-video", "https://www.calstatela.edu/accessibility/audio-and-video")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/vendor-requirements", "https://www.calstatela.edu/accessibility/vendor-requirements")</f>
         <v/>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -6233,7 +6233,7 @@
         <v>1</v>
       </c>
       <c r="H69" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I69" t="inlineStr">
         <is>
@@ -6262,7 +6262,7 @@
         </is>
       </c>
       <c r="O69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q69" t="n">
         <v>0</v>
@@ -6271,7 +6271,7 @@
         <v>0</v>
       </c>
       <c r="S69" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T69" t="inlineStr">
         <is>
@@ -6286,21 +6286,21 @@
     </row>
     <row r="70">
       <c r="A70" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B70" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/udoit", "https://www.calstatela.edu/accessibility/udoit")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/vendor-requirements", "https://www.calstatela.edu/accessibility/vendor-requirements")</f>
         <v/>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -6317,7 +6317,7 @@
         <v>1</v>
       </c>
       <c r="H70" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I70" t="inlineStr">
         <is>
@@ -6346,7 +6346,7 @@
         </is>
       </c>
       <c r="O70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q70" t="n">
         <v>0</v>
@@ -6355,7 +6355,7 @@
         <v>0</v>
       </c>
       <c r="S70" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T70" t="inlineStr">
         <is>
@@ -6370,21 +6370,21 @@
     </row>
     <row r="71">
       <c r="A71" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B71" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/udoit", "https://www.calstatela.edu/accessibility/udoit")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/submit-ict-par", "https://www.calstatela.edu/accessibility/submit-ict-par")</f>
         <v/>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -6401,7 +6401,7 @@
         <v>1</v>
       </c>
       <c r="H71" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I71" t="inlineStr">
         <is>
@@ -6430,7 +6430,7 @@
         </is>
       </c>
       <c r="O71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q71" t="n">
         <v>0</v>
@@ -6439,7 +6439,7 @@
         <v>0</v>
       </c>
       <c r="S71" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T71" t="inlineStr">
         <is>
@@ -6454,21 +6454,21 @@
     </row>
     <row r="72">
       <c r="A72" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B72" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/new-faculty", "https://www.calstatela.edu/accessibility/new-faculty")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/submit-ict-par", "https://www.calstatela.edu/accessibility/submit-ict-par")</f>
         <v/>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -6485,7 +6485,7 @@
         <v>1</v>
       </c>
       <c r="H72" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I72" t="inlineStr">
         <is>
@@ -6514,7 +6514,7 @@
         </is>
       </c>
       <c r="O72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q72" t="n">
         <v>0</v>
@@ -6523,7 +6523,7 @@
         <v>0</v>
       </c>
       <c r="S72" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T72" t="inlineStr">
         <is>
@@ -6538,21 +6538,21 @@
     </row>
     <row r="73">
       <c r="A73" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B73" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/new-faculty", "https://www.calstatela.edu/accessibility/new-faculty")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/pre-approved-ict", "https://www.calstatela.edu/accessibility/pre-approved-ict")</f>
         <v/>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -6569,7 +6569,7 @@
         <v>1</v>
       </c>
       <c r="H73" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I73" t="inlineStr">
         <is>
@@ -6598,7 +6598,7 @@
         </is>
       </c>
       <c r="O73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q73" t="n">
         <v>0</v>
@@ -6607,7 +6607,7 @@
         <v>0</v>
       </c>
       <c r="S73" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T73" t="inlineStr">
         <is>
@@ -6622,21 +6622,21 @@
     </row>
     <row r="74">
       <c r="A74" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B74" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/instructional-materials", "https://www.calstatela.edu/accessibility/instructional-materials")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/pre-approved-ict", "https://www.calstatela.edu/accessibility/pre-approved-ict")</f>
         <v/>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -6653,7 +6653,7 @@
         <v>1</v>
       </c>
       <c r="H74" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I74" t="inlineStr">
         <is>
@@ -6682,7 +6682,7 @@
         </is>
       </c>
       <c r="O74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q74" t="n">
         <v>0</v>
@@ -6691,7 +6691,7 @@
         <v>0</v>
       </c>
       <c r="S74" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T74" t="inlineStr">
         <is>
@@ -6706,21 +6706,21 @@
     </row>
     <row r="75">
       <c r="A75" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B75" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/instructional-materials", "https://www.calstatela.edu/accessibility/instructional-materials")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ict-purchase-approval-request-ict-par-walkthrough", "https://www.calstatela.edu/accessibility/ict-purchase-approval-request-ict-par-walkthrough")</f>
         <v/>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -6737,7 +6737,7 @@
         <v>1</v>
       </c>
       <c r="H75" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I75" t="inlineStr">
         <is>
@@ -6766,7 +6766,7 @@
         </is>
       </c>
       <c r="O75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q75" t="n">
         <v>0</v>
@@ -6775,7 +6775,7 @@
         <v>0</v>
       </c>
       <c r="S75" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T75" t="inlineStr">
         <is>
@@ -6790,21 +6790,21 @@
     </row>
     <row r="76">
       <c r="A76" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B76" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/seven-essential-skills-crafting-accessible-content", "https://www.calstatela.edu/accessibility/seven-essential-skills-crafting-accessible-content")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ict-purchase-approval-request-ict-par-walkthrough", "https://www.calstatela.edu/accessibility/ict-purchase-approval-request-ict-par-walkthrough")</f>
         <v/>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -6821,7 +6821,7 @@
         <v>1</v>
       </c>
       <c r="H76" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I76" t="inlineStr">
         <is>
@@ -6850,7 +6850,7 @@
         </is>
       </c>
       <c r="O76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q76" t="n">
         <v>0</v>
@@ -6859,7 +6859,7 @@
         <v>0</v>
       </c>
       <c r="S76" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T76" t="inlineStr">
         <is>
@@ -6874,21 +6874,21 @@
     </row>
     <row r="77">
       <c r="A77" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B77" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/seven-essential-skills-crafting-accessible-content", "https://www.calstatela.edu/accessibility/seven-essential-skills-crafting-accessible-content")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/acquiring-accessible-ict", "https://www.calstatela.edu/accessibility/acquiring-accessible-ict")</f>
         <v/>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -6905,7 +6905,7 @@
         <v>1</v>
       </c>
       <c r="H77" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I77" t="inlineStr">
         <is>
@@ -6934,7 +6934,7 @@
         </is>
       </c>
       <c r="O77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q77" t="n">
         <v>0</v>
@@ -6943,7 +6943,7 @@
         <v>0</v>
       </c>
       <c r="S77" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T77" t="inlineStr">
         <is>
@@ -6958,21 +6958,21 @@
     </row>
     <row r="78">
       <c r="A78" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B78" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/popetech-wave", "https://www.calstatela.edu/accessibility/popetech-wave")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/acquiring-accessible-ict", "https://www.calstatela.edu/accessibility/acquiring-accessible-ict")</f>
         <v/>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -6989,7 +6989,7 @@
         <v>1</v>
       </c>
       <c r="H78" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I78" t="inlineStr">
         <is>
@@ -7018,7 +7018,7 @@
         </is>
       </c>
       <c r="O78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q78" t="n">
         <v>0</v>
@@ -7027,7 +7027,7 @@
         <v>0</v>
       </c>
       <c r="S78" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T78" t="inlineStr">
         <is>
@@ -7042,21 +7042,21 @@
     </row>
     <row r="79">
       <c r="A79" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B79" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/popetech-wave", "https://www.calstatela.edu/accessibility/popetech-wave")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/zoom-and-teams", "https://www.calstatela.edu/accessibility/zoom-and-teams")</f>
         <v/>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -7073,7 +7073,7 @@
         <v>1</v>
       </c>
       <c r="H79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I79" t="inlineStr">
         <is>
@@ -7102,7 +7102,7 @@
         </is>
       </c>
       <c r="O79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q79" t="n">
         <v>0</v>
@@ -7111,7 +7111,7 @@
         <v>0</v>
       </c>
       <c r="S79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T79" t="inlineStr">
         <is>
@@ -7126,21 +7126,21 @@
     </row>
     <row r="80">
       <c r="A80" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B80" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/editoria11y-drupal", "https://www.calstatela.edu/accessibility/editoria11y-drupal")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/zoom-and-teams", "https://www.calstatela.edu/accessibility/zoom-and-teams")</f>
         <v/>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -7157,7 +7157,7 @@
         <v>1</v>
       </c>
       <c r="H80" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I80" t="inlineStr">
         <is>
@@ -7186,7 +7186,7 @@
         </is>
       </c>
       <c r="O80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q80" t="n">
         <v>0</v>
@@ -7195,7 +7195,7 @@
         <v>0</v>
       </c>
       <c r="S80" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T80" t="inlineStr">
         <is>
@@ -7210,21 +7210,21 @@
     </row>
     <row r="81">
       <c r="A81" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B81" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/editoria11y-drupal", "https://www.calstatela.edu/accessibility/editoria11y-drupal")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/qualtrics", "https://www.calstatela.edu/accessibility/qualtrics")</f>
         <v/>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -7241,7 +7241,7 @@
         <v>1</v>
       </c>
       <c r="H81" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I81" t="inlineStr">
         <is>
@@ -7270,7 +7270,7 @@
         </is>
       </c>
       <c r="O81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q81" t="n">
         <v>0</v>
@@ -7279,7 +7279,7 @@
         <v>0</v>
       </c>
       <c r="S81" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T81" t="inlineStr">
         <is>
@@ -7294,21 +7294,21 @@
     </row>
     <row r="82">
       <c r="A82" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B82" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web-accessibility-guidelines", "https://www.calstatela.edu/accessibility/web-accessibility-guidelines")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/qualtrics", "https://www.calstatela.edu/accessibility/qualtrics")</f>
         <v/>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -7325,7 +7325,7 @@
         <v>1</v>
       </c>
       <c r="H82" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I82" t="inlineStr">
         <is>
@@ -7354,7 +7354,7 @@
         </is>
       </c>
       <c r="O82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q82" t="n">
         <v>0</v>
@@ -7363,7 +7363,7 @@
         <v>0</v>
       </c>
       <c r="S82" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T82" t="inlineStr">
         <is>
@@ -7378,21 +7378,21 @@
     </row>
     <row r="83">
       <c r="A83" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B83" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web-accessibility-guidelines", "https://www.calstatela.edu/accessibility/web-accessibility-guidelines")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/social-media", "https://www.calstatela.edu/accessibility/social-media")</f>
         <v/>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -7409,7 +7409,7 @@
         <v>1</v>
       </c>
       <c r="H83" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I83" t="inlineStr">
         <is>
@@ -7438,7 +7438,7 @@
         </is>
       </c>
       <c r="O83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q83" t="n">
         <v>0</v>
@@ -7447,7 +7447,7 @@
         <v>0</v>
       </c>
       <c r="S83" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T83" t="inlineStr">
         <is>
@@ -7462,21 +7462,21 @@
     </row>
     <row r="84">
       <c r="A84" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B84" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web-accessibility-liaisons", "https://www.calstatela.edu/accessibility/web-accessibility-liaisons")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/social-media", "https://www.calstatela.edu/accessibility/social-media")</f>
         <v/>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -7493,7 +7493,7 @@
         <v>1</v>
       </c>
       <c r="H84" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I84" t="inlineStr">
         <is>
@@ -7522,7 +7522,7 @@
         </is>
       </c>
       <c r="O84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q84" t="n">
         <v>0</v>
@@ -7531,7 +7531,7 @@
         <v>0</v>
       </c>
       <c r="S84" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T84" t="inlineStr">
         <is>
@@ -7546,21 +7546,21 @@
     </row>
     <row r="85">
       <c r="A85" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B85" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web-accessibility-liaisons", "https://www.calstatela.edu/accessibility/web-accessibility-liaisons")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessibility-statement", "https://www.calstatela.edu/accessibility/accessibility-statement")</f>
         <v/>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -7577,7 +7577,7 @@
         <v>1</v>
       </c>
       <c r="H85" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I85" t="inlineStr">
         <is>
@@ -7606,7 +7606,7 @@
         </is>
       </c>
       <c r="O85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q85" t="n">
         <v>0</v>
@@ -7615,7 +7615,7 @@
         <v>0</v>
       </c>
       <c r="S85" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T85" t="inlineStr">
         <is>
@@ -7630,21 +7630,21 @@
     </row>
     <row r="86">
       <c r="A86" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B86" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ramp", "https://www.calstatela.edu/accessibility/ramp")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessibility-statement", "https://www.calstatela.edu/accessibility/accessibility-statement")</f>
         <v/>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -7661,7 +7661,7 @@
         <v>1</v>
       </c>
       <c r="H86" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I86" t="inlineStr">
         <is>
@@ -7690,7 +7690,7 @@
         </is>
       </c>
       <c r="O86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q86" t="n">
         <v>0</v>
@@ -7699,7 +7699,7 @@
         <v>0</v>
       </c>
       <c r="S86" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T86" t="inlineStr">
         <is>
@@ -7714,21 +7714,21 @@
     </row>
     <row r="87">
       <c r="A87" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B87" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/ramp", "https://www.calstatela.edu/accessibility/ramp")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/frequently-asked-questions", "https://www.calstatela.edu/accessibility/frequently-asked-questions")</f>
         <v/>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -7745,7 +7745,7 @@
         <v>1</v>
       </c>
       <c r="H87" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I87" t="inlineStr">
         <is>
@@ -7774,7 +7774,7 @@
         </is>
       </c>
       <c r="O87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q87" t="n">
         <v>0</v>
@@ -7783,7 +7783,7 @@
         <v>0</v>
       </c>
       <c r="S87" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T87" t="inlineStr">
         <is>
@@ -7798,21 +7798,21 @@
     </row>
     <row r="88">
       <c r="A88" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B88" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web", "https://www.calstatela.edu/accessibility/web")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/frequently-asked-questions", "https://www.calstatela.edu/accessibility/frequently-asked-questions")</f>
         <v/>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -7829,7 +7829,7 @@
         <v>1</v>
       </c>
       <c r="H88" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I88" t="inlineStr">
         <is>
@@ -7858,7 +7858,7 @@
         </is>
       </c>
       <c r="O88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q88" t="n">
         <v>0</v>
@@ -7867,7 +7867,7 @@
         <v>0</v>
       </c>
       <c r="S88" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T88" t="inlineStr">
         <is>
@@ -7882,21 +7882,21 @@
     </row>
     <row r="89">
       <c r="A89" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
         <v/>
       </c>
       <c r="B89" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/web", "https://www.calstatela.edu/accessibility/web")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/campus-resources", "https://www.calstatela.edu/accessibility/campus-resources")</f>
         <v/>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>769f4a</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -7913,7 +7913,7 @@
         <v>1</v>
       </c>
       <c r="H89" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I89" t="inlineStr">
         <is>
@@ -7942,7 +7942,7 @@
         </is>
       </c>
       <c r="O89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q89" t="n">
         <v>0</v>
@@ -7951,7 +7951,7 @@
         <v>0</v>
       </c>
       <c r="S89" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T89" t="inlineStr">
         <is>
@@ -7966,21 +7966,21 @@
     </row>
     <row r="90">
       <c r="A90" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Annual%20Security%20Report.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
         <v/>
       </c>
       <c r="B90" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/services", "https://www.calstatela.edu/accessibility/services")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/campus-resources", "https://www.calstatela.edu/accessibility/campus-resources")</f>
         <v/>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:18</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>769f4a</t>
+          <t>c73bc1</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -7997,7 +7997,7 @@
         <v>1</v>
       </c>
       <c r="H90" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I90" t="inlineStr">
         <is>
@@ -8026,7 +8026,7 @@
         </is>
       </c>
       <c r="O90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q90" t="n">
         <v>0</v>
@@ -8035,7 +8035,7 @@
         <v>0</v>
       </c>
       <c r="S90" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T90" t="inlineStr">
         <is>
@@ -8050,21 +8050,21 @@
     </row>
     <row r="91">
       <c r="A91" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf", "https://www.calstatela.edu/sites/default/files/2025%20Campus%20Safety%20Plan.pdf")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/sites/default/files/ati_handout_021721.pdf", "https://www.calstatela.edu/sites/default/files/ati_handout_021721.pdf")</f>
         <v/>
       </c>
       <c r="B91" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/services", "https://www.calstatela.edu/accessibility/services")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessibility-primer", "https://www.calstatela.edu/accessibility/accessibility-primer")</f>
         <v/>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:21</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>c73bc1</t>
+          <t>9f5e7f</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -8106,11 +8106,11 @@
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q91" t="n">
         <v>0</v>
@@ -8138,12 +8138,12 @@
         <v/>
       </c>
       <c r="B92" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/report-accessibility-issue", "https://www.calstatela.edu/accessibility/report-accessibility-issue")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessibility-primer", "https://www.calstatela.edu/accessibility/accessibility-primer")</f>
         <v/>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:21</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -8222,12 +8222,12 @@
         <v/>
       </c>
       <c r="B93" s="1">
-        <f>HYPERLINK("https://www.calstatela.edu/accessibility/report-accessibility-issue", "https://www.calstatela.edu/accessibility/report-accessibility-issue")</f>
+        <f>HYPERLINK("https://www.calstatela.edu/accessibility/accessibility-primer", "https://www.calstatela.edu/accessibility/accessibility-primer")</f>
         <v/>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2025-11-03 20:05:03</t>
+          <t>2025-12-16 19:10:21</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">

</xml_diff>